<commit_message>
Added passenger information to sheet.
</commit_message>
<xml_diff>
--- a/Jan2016MetaCrunch.xlsx
+++ b/Jan2016MetaCrunch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="Jan2016MetaCrunch" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t xml:space="preserve">Total Taxi Count: </t>
   </si>
@@ -105,13 +105,22 @@
   <si>
     <t>Midtown&lt;-&gt;Upper East Side&lt;-&gt;Midtown</t>
   </si>
+  <si>
+    <t>Total Passengers:</t>
+  </si>
+  <si>
+    <t>Passengers/Carpool:</t>
+  </si>
+  <si>
+    <t>Upper East Side All</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -597,7 +606,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -742,7 +751,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Jan2016MetaCrunch!$B$14</c:f>
+              <c:f>Jan2016MetaCrunch!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -766,11 +775,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Jan2016MetaCrunch!$C$13:$H$13</c15:sqref>
+                    <c15:sqref>Jan2016MetaCrunch!$C$14:$H$14</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Jan2016MetaCrunch!$C$13:$F$13</c:f>
+              <c:f>Jan2016MetaCrunch!$C$14:$F$14</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -793,11 +802,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Jan2016MetaCrunch!$C$14:$H$14</c15:sqref>
+                    <c15:sqref>Jan2016MetaCrunch!$C$15:$H$15</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Jan2016MetaCrunch!$C$14:$F$14</c:f>
+              <c:f>Jan2016MetaCrunch!$C$15:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -827,7 +836,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Jan2016MetaCrunch!$B$15</c:f>
+              <c:f>Jan2016MetaCrunch!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -851,11 +860,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Jan2016MetaCrunch!$C$13:$H$13</c15:sqref>
+                    <c15:sqref>Jan2016MetaCrunch!$C$14:$H$14</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Jan2016MetaCrunch!$C$13:$F$13</c:f>
+              <c:f>Jan2016MetaCrunch!$C$14:$F$14</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -878,11 +887,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Jan2016MetaCrunch!$C$15:$H$15</c15:sqref>
+                    <c15:sqref>Jan2016MetaCrunch!$C$16:$H$16</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Jan2016MetaCrunch!$C$15:$F$15</c:f>
+              <c:f>Jan2016MetaCrunch!$C$16:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1250,7 +1259,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Jan2016MetaCrunch!$B$14</c:f>
+              <c:f>Jan2016MetaCrunch!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1274,11 +1283,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Jan2016MetaCrunch!$C$13:$H$13</c15:sqref>
+                    <c15:sqref>Jan2016MetaCrunch!$C$14:$H$14</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Jan2016MetaCrunch!$G$13:$H$13</c:f>
+              <c:f>Jan2016MetaCrunch!$G$14:$H$14</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1295,11 +1304,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Jan2016MetaCrunch!$C$14:$H$14</c15:sqref>
+                    <c15:sqref>Jan2016MetaCrunch!$C$15:$H$15</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Jan2016MetaCrunch!$G$14:$H$14</c:f>
+              <c:f>Jan2016MetaCrunch!$G$15:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1323,7 +1332,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Jan2016MetaCrunch!$B$15</c:f>
+              <c:f>Jan2016MetaCrunch!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1347,11 +1356,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Jan2016MetaCrunch!$C$13:$H$13</c15:sqref>
+                    <c15:sqref>Jan2016MetaCrunch!$C$14:$H$14</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Jan2016MetaCrunch!$G$13:$H$13</c:f>
+              <c:f>Jan2016MetaCrunch!$G$14:$H$14</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1368,11 +1377,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Jan2016MetaCrunch!$C$15:$H$15</c15:sqref>
+                    <c15:sqref>Jan2016MetaCrunch!$C$16:$H$16</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Jan2016MetaCrunch!$G$15:$H$15</c:f>
+              <c:f>Jan2016MetaCrunch!$G$16:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3069,7 +3078,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2820000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+          <a:bodyPr rot="-2820000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="t" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -9813,14 +9822,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
@@ -9858,6 +9868,9 @@
       <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="O1" s="1"/>
@@ -9908,6 +9921,10 @@
       <c r="I3">
         <v>43614</v>
       </c>
+      <c r="J3">
+        <f>SUM(G3:I3)</f>
+        <v>136626</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -9934,6 +9951,10 @@
       <c r="I4">
         <v>22849</v>
       </c>
+      <c r="J4">
+        <f>SUM(G4:I4)</f>
+        <v>72371</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -9959,6 +9980,10 @@
       </c>
       <c r="I6">
         <v>0.52</v>
+      </c>
+      <c r="J6">
+        <f>J4/J3</f>
+        <v>0.52970152094037737</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -9987,6 +10012,10 @@
       <c r="I7">
         <v>43923.16</v>
       </c>
+      <c r="J7">
+        <f>SUM(G7:I7)</f>
+        <v>104137.56</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -10013,6 +10042,10 @@
       <c r="I8">
         <v>19.899999999999999</v>
       </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J11" si="0">SUM(G8:I8)</f>
+        <v>47.18</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -10039,6 +10072,10 @@
       <c r="I9">
         <v>421993.52</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>1155845.05</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -10065,75 +10102,153 @@
       <c r="I10">
         <v>1.65</v>
       </c>
+      <c r="J10">
+        <f>J11/J3</f>
+        <v>1.6405983487769533</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>27</v>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <f>B3*B10</f>
+        <v>36728.800000000003</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:G11" si="1">C3*C10</f>
+        <v>40451.9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>47516.22</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>162155.52000000002</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>82821.75</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11" si="2">H3*H10</f>
+        <v>69363.540000000008</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11" si="3">I3*I10</f>
+        <v>71963.099999999991</v>
+      </c>
+      <c r="J11">
+        <f>SUM(G11:I11)</f>
+        <v>224148.39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <f>B11/B4</f>
+        <v>3.1753090689029135</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:G12" si="4">C11/C4</f>
+        <v>2.2943622029380069</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="4"/>
+        <v>2.3247820343461032</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
+        <v>2.427732247391194</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>3.0430153947900211</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12" si="5">H11/H4</f>
+        <v>3.1097753866846003</v>
+      </c>
+      <c r="I12">
+        <f>I11/I4</f>
+        <v>3.1495076370957151</v>
+      </c>
+      <c r="J12">
+        <f>J11/J4</f>
+        <v>3.0972128338699205</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14">
-        <v>23696</v>
-      </c>
-      <c r="D14">
-        <f>D3+C3</f>
-        <v>55429</v>
-      </c>
-      <c r="E14">
-        <v>50195</v>
-      </c>
-      <c r="F14">
-        <f>I3+H3</f>
-        <v>86431</v>
-      </c>
-      <c r="G14">
-        <v>100096</v>
-      </c>
-      <c r="H14">
-        <f>SUM(G3:I3)</f>
-        <v>136626</v>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>23696</v>
+      </c>
+      <c r="D15">
+        <f>D3+C3</f>
+        <v>55429</v>
+      </c>
+      <c r="E15">
+        <v>50195</v>
+      </c>
+      <c r="F15">
+        <f>I3+H3</f>
+        <v>86431</v>
+      </c>
+      <c r="G15">
+        <v>100096</v>
+      </c>
+      <c r="H15">
+        <f>SUM(G3:I3)</f>
+        <v>136626</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>11567</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <f>D4+C4</f>
         <v>38070</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>27217</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <f>I4+H4</f>
         <v>45154</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>66793</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <f>SUM(G4:I4)</f>
         <v>72371</v>
       </c>
@@ -10148,7 +10263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I10" workbookViewId="0">
       <selection activeCell="N100" sqref="N100"/>
     </sheetView>
   </sheetViews>

</xml_diff>